<commit_message>
Files before bekef from laptop
</commit_message>
<xml_diff>
--- a/events/Caesaria_2023/StartList_Additions.xlsx
+++ b/events/Caesaria_2023/StartList_Additions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
   <si>
     <t xml:space="preserve">STNO</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">עמק חפר</t>
   </si>
   <si>
-    <t xml:space="preserve">קצר </t>
+    <t xml:space="preserve">קצר</t>
   </si>
   <si>
     <t xml:space="preserve">נוער עמק חפר</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">ברק שדמה</t>
   </si>
   <si>
-    <t xml:space="preserve">קצרצר </t>
+    <t xml:space="preserve">קצרצר</t>
   </si>
   <si>
     <t xml:space="preserve">איל ויסר</t>
@@ -148,13 +148,37 @@
     <t xml:space="preserve">נטע באר</t>
   </si>
   <si>
+    <t xml:space="preserve">כרמי מעיין</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לב השרון</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חגי לדרר</t>
+  </si>
+  <si>
+    <t xml:space="preserve">יעקבסון ארד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">וקס אחא</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פישר נעם</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מעוז תבור</t>
+  </si>
+  <si>
+    <t xml:space="preserve">צוקרמן יותם</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מרשון נגה</t>
+  </si>
+  <si>
     <t xml:space="preserve">ורבין עידן</t>
   </si>
   <si>
-    <t xml:space="preserve">האיגוד</t>
-  </si>
-  <si>
-    <t xml:space="preserve">קצר</t>
+    <t xml:space="preserve">אסא תא</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
@@ -178,6 +202,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">מספר צ</t>
     </r>
@@ -197,6 +222,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">יפ </t>
     </r>
@@ -223,7 +249,7 @@
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -235,16 +261,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="177"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="177"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="177"/>
     </font>
     <font>
       <sz val="11"/>
@@ -259,12 +288,6 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,14 +373,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,14 +395,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="24:24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,7 +452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>6796</v>
       </c>
@@ -470,7 +485,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>6930</v>
       </c>
@@ -503,7 +518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>7006</v>
       </c>
@@ -536,7 +551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>7015</v>
       </c>
@@ -569,7 +584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>7018</v>
       </c>
@@ -602,7 +617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>7016</v>
       </c>
@@ -635,7 +650,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7017</v>
       </c>
@@ -645,7 +660,7 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="6" t="n">
@@ -659,7 +674,7 @@
       <c r="M8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>7081</v>
       </c>
@@ -692,7 +707,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>7082</v>
       </c>
@@ -725,7 +740,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>7137</v>
       </c>
@@ -758,7 +773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>111111111</v>
       </c>
@@ -789,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>111111112</v>
       </c>
@@ -820,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>111111113</v>
       </c>
@@ -851,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>111111114</v>
       </c>
@@ -861,7 +876,7 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="6" t="n">
@@ -881,106 +896,297 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>111111115</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>111111116</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>5673</v>
+        <v>111111117</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="6" t="n">
+      <c r="K18" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>111111118</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>111111119</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>111111120</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>111111121</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K22" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>5673</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="1" t="n">
+      <c r="F23" s="3"/>
+      <c r="G23" s="1" t="n">
         <v>2071500</v>
       </c>
-      <c r="H18" s="9" t="b">
+      <c r="H23" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="0"/>
-      <c r="K18" s="9" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="I23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="9" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
         <v>346305691</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="6" t="n">
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="6" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="0" t="n">
+      <c r="F24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <v>206790</v>
       </c>
-      <c r="H23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="M23" s="0" t="n">
+      <c r="H24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="N23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="O23" s="0" t="n">
+      <c r="N24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O24" s="1" t="n">
         <v>538470469</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="J28" s="0"/>
+    </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="J33" s="0"/>
+    </row>
     <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>